<commit_message>
motor boat and lench finished. working on radioactive tower attack and button intractivity for them
</commit_message>
<xml_diff>
--- a/SeaWar info/تجهیزات کمیاب.xlsx
+++ b/SeaWar info/تجهیزات کمیاب.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342C2158-55C7-4FC3-88E0-E88BF22C495E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -165,13 +166,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -183,6 +184,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -231,7 +235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,9 +268,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,6 +320,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -474,49 +512,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="26.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="26.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="48.21875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="25.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="48.28515625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -557,7 +595,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -598,7 +636,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -637,7 +675,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -676,7 +714,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -715,7 +753,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -754,7 +792,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -793,7 +831,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -832,7 +870,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -871,7 +909,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -910,7 +948,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -949,7 +987,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -988,7 +1026,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -998,24 +1036,24 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -1056,14 +1094,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>1</v>
       </c>
       <c r="B18" s="5">
         <v>0</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>1.2</v>
       </c>
       <c r="D18" s="5">
@@ -1097,14 +1135,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>2</v>
       </c>
       <c r="B19" s="5">
         <v>0</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>1.3</v>
       </c>
       <c r="D19" s="3">
@@ -1137,14 +1175,14 @@
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>3</v>
       </c>
       <c r="B20" s="5">
         <v>0</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>1.4</v>
       </c>
       <c r="D20" s="3">
@@ -1177,14 +1215,14 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>4</v>
       </c>
       <c r="B21" s="5">
         <v>0</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>1.5</v>
       </c>
       <c r="D21" s="3">
@@ -1217,14 +1255,14 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>5</v>
       </c>
       <c r="B22" s="5">
         <v>0</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>1.6</v>
       </c>
       <c r="D22" s="3">
@@ -1257,14 +1295,14 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>6</v>
       </c>
       <c r="B23" s="5">
         <v>0</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>1.7</v>
       </c>
       <c r="D23" s="3">
@@ -1297,14 +1335,14 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>7</v>
       </c>
       <c r="B24" s="5">
         <v>0</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>1.8</v>
       </c>
       <c r="D24" s="3">
@@ -1337,14 +1375,14 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>8</v>
       </c>
       <c r="B25" s="5">
         <v>0</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>1.9</v>
       </c>
       <c r="D25" s="3">
@@ -1377,14 +1415,14 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>9</v>
       </c>
       <c r="B26" s="5">
         <v>0</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="7">
         <v>2</v>
       </c>
       <c r="D26" s="3">
@@ -1417,14 +1455,14 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>10</v>
       </c>
       <c r="B27" s="5">
         <v>0</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="7">
         <v>2.1</v>
       </c>
       <c r="D27" s="3">
@@ -1457,14 +1495,14 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>11</v>
       </c>
       <c r="B28" s="5">
         <v>0</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="7">
         <v>2.2000000000000002</v>
       </c>
       <c r="D28" s="3">
@@ -1497,7 +1535,7 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
@@ -1512,24 +1550,24 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>6</v>
       </c>
@@ -1570,14 +1608,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>1</v>
       </c>
       <c r="B32" s="5">
         <v>0</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <v>0.8</v>
       </c>
       <c r="D32" s="5">
@@ -1611,14 +1649,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>2</v>
       </c>
       <c r="B33" s="5">
         <v>0</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="8">
         <f>C32-0.03</f>
         <v>0.77</v>
       </c>
@@ -1652,14 +1690,14 @@
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>3</v>
       </c>
       <c r="B34" s="5">
         <v>0</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="8">
         <f t="shared" ref="C34:C42" si="7">C33-0.03</f>
         <v>0.74</v>
       </c>
@@ -1693,14 +1731,14 @@
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>4</v>
       </c>
       <c r="B35" s="5">
         <v>0</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8">
         <f t="shared" si="7"/>
         <v>0.71</v>
       </c>
@@ -1734,14 +1772,14 @@
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>5</v>
       </c>
       <c r="B36" s="5">
         <v>0</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="8">
         <f t="shared" si="7"/>
         <v>0.67999999999999994</v>
       </c>
@@ -1775,14 +1813,14 @@
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>6</v>
       </c>
       <c r="B37" s="5">
         <v>0</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="8">
         <f t="shared" si="7"/>
         <v>0.64999999999999991</v>
       </c>
@@ -1816,14 +1854,14 @@
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>7</v>
       </c>
       <c r="B38" s="5">
         <v>0</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="8">
         <f t="shared" si="7"/>
         <v>0.61999999999999988</v>
       </c>
@@ -1857,14 +1895,14 @@
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>8</v>
       </c>
       <c r="B39" s="5">
         <v>0</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="8">
         <f t="shared" si="7"/>
         <v>0.58999999999999986</v>
       </c>
@@ -1898,14 +1936,14 @@
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>9</v>
       </c>
       <c r="B40" s="5">
         <v>0</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="8">
         <f t="shared" si="7"/>
         <v>0.55999999999999983</v>
       </c>
@@ -1939,14 +1977,14 @@
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>10</v>
       </c>
       <c r="B41" s="5">
         <v>0</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="8">
         <f t="shared" si="7"/>
         <v>0.5299999999999998</v>
       </c>
@@ -1980,14 +2018,14 @@
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>11</v>
       </c>
       <c r="B42" s="5">
         <v>0</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="8">
         <f t="shared" si="7"/>
         <v>0.49999999999999978</v>
       </c>
@@ -2021,7 +2059,7 @@
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="3"/>
@@ -2036,24 +2074,24 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>6</v>
       </c>
@@ -2094,7 +2132,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>1</v>
       </c>
@@ -2135,7 +2173,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>2</v>
       </c>
@@ -2176,7 +2214,7 @@
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>3</v>
       </c>
@@ -2217,7 +2255,7 @@
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>4</v>
       </c>
@@ -2258,7 +2296,7 @@
       <c r="L49" s="5"/>
       <c r="M49" s="5"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>5</v>
       </c>
@@ -2299,7 +2337,7 @@
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>6</v>
       </c>
@@ -2340,7 +2378,7 @@
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>7</v>
       </c>
@@ -2381,7 +2419,7 @@
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>8</v>
       </c>
@@ -2422,7 +2460,7 @@
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>9</v>
       </c>
@@ -2463,7 +2501,7 @@
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>10</v>
       </c>
@@ -2504,7 +2542,7 @@
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>11</v>
       </c>
@@ -2545,7 +2583,7 @@
       <c r="L56" s="5"/>
       <c r="M56" s="5"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2560,7 +2598,7 @@
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="3"/>
@@ -2575,7 +2613,7 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="3"/>
@@ -2590,7 +2628,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="3"/>
@@ -2605,7 +2643,7 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="3"/>
@@ -2620,7 +2658,7 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="3"/>
@@ -2635,7 +2673,7 @@
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="3"/>
@@ -2650,7 +2688,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="3"/>
@@ -2665,7 +2703,7 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="3"/>
@@ -2680,7 +2718,7 @@
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="3"/>
@@ -2695,7 +2733,7 @@
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="3"/>
@@ -2710,7 +2748,7 @@
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="3"/>
@@ -2725,7 +2763,7 @@
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="3"/>
@@ -2740,7 +2778,7 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="3"/>
@@ -2755,7 +2793,7 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="3"/>
@@ -2770,7 +2808,7 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="3"/>
@@ -2785,7 +2823,7 @@
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -2800,7 +2838,7 @@
       <c r="L74" s="6"/>
       <c r="M74" s="6"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2815,7 +2853,7 @@
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="3"/>
@@ -2830,7 +2868,7 @@
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="3"/>
@@ -2845,7 +2883,7 @@
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="3"/>
@@ -2860,7 +2898,7 @@
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="3"/>
@@ -2875,7 +2913,7 @@
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="3"/>
@@ -2890,7 +2928,7 @@
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="3"/>
@@ -2905,7 +2943,7 @@
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="3"/>
@@ -2920,7 +2958,7 @@
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="3"/>
@@ -2935,7 +2973,7 @@
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="3"/>
@@ -2950,7 +2988,7 @@
       <c r="L84" s="2"/>
       <c r="M84" s="2"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="3"/>
@@ -2965,7 +3003,7 @@
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="3"/>
@@ -2980,7 +3018,7 @@
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="3"/>
@@ -2995,7 +3033,7 @@
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="3"/>
@@ -3010,7 +3048,7 @@
       <c r="L88" s="2"/>
       <c r="M88" s="2"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="3"/>
@@ -3025,7 +3063,7 @@
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="3"/>
@@ -3040,7 +3078,7 @@
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="3"/>
@@ -3055,7 +3093,7 @@
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="3"/>
@@ -3070,7 +3108,7 @@
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="3"/>
@@ -3085,7 +3123,7 @@
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="3"/>
@@ -3100,7 +3138,7 @@
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="3"/>
@@ -3115,7 +3153,7 @@
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="3"/>
@@ -3130,7 +3168,7 @@
       <c r="L96" s="2"/>
       <c r="M96" s="2"/>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -3145,7 +3183,7 @@
       <c r="L98" s="6"/>
       <c r="M98" s="6"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3160,7 +3198,7 @@
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="3"/>
@@ -3175,7 +3213,7 @@
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="3"/>
@@ -3190,7 +3228,7 @@
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="3"/>
@@ -3205,7 +3243,7 @@
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="3"/>
@@ -3220,7 +3258,7 @@
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="3"/>
@@ -3235,7 +3273,7 @@
       <c r="L104" s="2"/>
       <c r="M104" s="2"/>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="3"/>
@@ -3250,7 +3288,7 @@
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="3"/>
@@ -3265,7 +3303,7 @@
       <c r="L106" s="2"/>
       <c r="M106" s="2"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="3"/>
@@ -3280,7 +3318,7 @@
       <c r="L107" s="2"/>
       <c r="M107" s="2"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="3"/>
@@ -3295,7 +3333,7 @@
       <c r="L108" s="2"/>
       <c r="M108" s="2"/>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="3"/>
@@ -3310,7 +3348,7 @@
       <c r="L109" s="2"/>
       <c r="M109" s="2"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="3"/>
@@ -3325,7 +3363,7 @@
       <c r="L110" s="2"/>
       <c r="M110" s="2"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="3"/>
@@ -3340,7 +3378,7 @@
       <c r="L111" s="2"/>
       <c r="M111" s="2"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="3"/>
@@ -3355,7 +3393,7 @@
       <c r="L112" s="2"/>
       <c r="M112" s="2"/>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="3"/>
@@ -3370,7 +3408,7 @@
       <c r="L113" s="2"/>
       <c r="M113" s="2"/>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="3"/>
@@ -3385,7 +3423,7 @@
       <c r="L114" s="2"/>
       <c r="M114" s="2"/>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="3"/>
@@ -3400,7 +3438,7 @@
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="3"/>
@@ -3415,7 +3453,7 @@
       <c r="L116" s="2"/>
       <c r="M116" s="2"/>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="3"/>
@@ -3430,7 +3468,7 @@
       <c r="L117" s="2"/>
       <c r="M117" s="2"/>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="3"/>
@@ -3445,7 +3483,7 @@
       <c r="L118" s="2"/>
       <c r="M118" s="2"/>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="3"/>
@@ -3460,7 +3498,7 @@
       <c r="L119" s="2"/>
       <c r="M119" s="2"/>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="3"/>
@@ -3488,24 +3526,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wrong spawn position bugs fixed, UI bugs remain, refactor code for removing codes about using layer, working on electric tower
</commit_message>
<xml_diff>
--- a/SeaWar info/تجهیزات کمیاب.xlsx
+++ b/SeaWar info/تجهیزات کمیاب.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342C2158-55C7-4FC3-88E0-E88BF22C495E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA3DD8E-A253-4774-9B17-CB326295AC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -515,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>

</xml_diff>